<commit_message>
Updated embed page generator
</commit_message>
<xml_diff>
--- a/samples/PowerBi/EmbedYourPBIApp/PBIPayloadGenerator/input.xlsx
+++ b/samples/PowerBi/EmbedYourPBIApp/PBIPayloadGenerator/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\PBIPayloadGenerator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ys\Git\Other\BCTech\samples\PowerBi\EmbedYourPBIApp\PBIPayloadGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9A6577-19BC-46D5-9558-C6B9BFF502B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472A96AD-1205-4F19-8B15-85B95018EE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBIReports" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -130,6 +130,27 @@
   </si>
   <si>
     <t>Profitability</t>
+  </si>
+  <si>
+    <t>PBIReportPage</t>
+  </si>
+  <si>
+    <t>ReportSection2fa580b0181e8c981cdc</t>
+  </si>
+  <si>
+    <t>ReportSectionf72eb4d7e5e35db3b283</t>
+  </si>
+  <si>
+    <t>ReportSection6a30609896651f006f0f</t>
+  </si>
+  <si>
+    <t>ReportSection64d670dfa9da1a5b7033</t>
+  </si>
+  <si>
+    <t>ReportSection6838cf9cda361d088e0a</t>
+  </si>
+  <si>
+    <t>ReportSectionbb4917d9edb6d427282c</t>
   </si>
 </sst>
 </file>
@@ -468,26 +489,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.76171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.9375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.29296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5859375" customWidth="1"/>
-    <col min="5" max="5" width="41.41015625" customWidth="1"/>
-    <col min="6" max="6" width="51.703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.17578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" customWidth="1"/>
+    <col min="6" max="6" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" customWidth="1"/>
+    <col min="9" max="9" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -512,8 +534,11 @@
       <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+      <c r="I1" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>50100</v>
       </c>
@@ -541,8 +566,11 @@
       <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+      <c r="I2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>50101</v>
       </c>
@@ -570,8 +598,11 @@
       <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+      <c r="I3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>50102</v>
       </c>
@@ -599,8 +630,11 @@
       <c r="H4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+      <c r="I4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>50103</v>
       </c>
@@ -628,8 +662,11 @@
       <c r="H5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+      <c r="I5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>50104</v>
       </c>
@@ -657,8 +694,11 @@
       <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="43" x14ac:dyDescent="0.5">
+      <c r="I6" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>50105</v>
       </c>
@@ -686,9 +726,12 @@
       <c r="H7" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I7" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -703,17 +746,17 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.76171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.05859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.1171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.8203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.9375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="64.17578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -733,7 +776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>50140</v>
       </c>
@@ -763,20 +806,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279D5BCD-102B-4F28-B1A5-95C97D1C61B4}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="26.05859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.1171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.64453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="65" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -793,12 +836,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="str">
-        <f>_xlfn.CONCAT("PBI",SUBSTITUTE(C2," ",""))</f>
+        <f t="shared" ref="B2:B7" si="0">_xlfn.CONCAT("PBI",SUBSTITUTE(C2," ",""))</f>
         <v>PBIFinancialOverview</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -812,95 +855,95 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f>_xlfn.CONCAT("PBI",SUBSTITUTE(C3," ",""))</f>
+        <f t="shared" si="0"/>
         <v>PBIIncomeStatementbyMonth</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D7" si="0">B3</f>
+        <f t="shared" ref="D3:D7" si="1">B3</f>
         <v>PBIIncomeStatementbyMonth</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2" t="str">
-        <f>_xlfn.CONCAT("PBI",SUBSTITUTE(C4," ",""))</f>
+        <f t="shared" si="0"/>
         <v>PBIBalanceSheetbyMonth</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PBIBalanceSheetbyMonth</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="2" t="str">
-        <f>_xlfn.CONCAT("PBI",SUBSTITUTE(C5," ",""))</f>
+        <f t="shared" si="0"/>
         <v>PBIBudgetComparison</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PBIBudgetComparison</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="str">
-        <f>_xlfn.CONCAT("PBI",SUBSTITUTE(C6," ",""))</f>
+        <f t="shared" si="0"/>
         <v>PBILiquidityKPIs</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PBILiquidityKPIs</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="str">
-        <f>_xlfn.CONCAT("PBI",SUBSTITUTE(C7," ",""))</f>
+        <f t="shared" si="0"/>
         <v>PBIProfitability</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>PBIProfitability</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -915,6 +958,7 @@
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{85ca8af4-763a-45c2-80ae-a5ca1b80bddc}" enabled="1" method="Standard" siteId="{06cdaf09-14f0-4cd1-8ac0-7bfed707a82c}" contentBits="0" removed="0"/>
   <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>

<commit_message>
PBI embed permission set generation
</commit_message>
<xml_diff>
--- a/samples/PowerBi/EmbedYourPBIApp/PBIPayloadGenerator/input.xlsx
+++ b/samples/PowerBi/EmbedYourPBIApp/PBIPayloadGenerator/input.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ys\Git\Other\BCTech\samples\PowerBi\EmbedYourPBIApp\PBIPayloadGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472A96AD-1205-4F19-8B15-85B95018EE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E347892F-CBF3-4AF0-946A-696B364DAA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11796" yWindow="17172" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBIReports" sheetId="1" r:id="rId1"/>
     <sheet name="RCExtensions" sheetId="2" r:id="rId2"/>
     <sheet name="RCExtensionActions" sheetId="3" r:id="rId3"/>
+    <sheet name="PermissionSets" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PBIReports!$A$1:$H$1</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -151,6 +152,15 @@
   </si>
   <si>
     <t>ReportSectionbb4917d9edb6d427282c</t>
+  </si>
+  <si>
+    <t>PBI EMBED VIEW</t>
+  </si>
+  <si>
+    <t>PBI Embed - View</t>
+  </si>
+  <si>
+    <t>PBIEmbedView.PermissionSet</t>
   </si>
 </sst>
 </file>
@@ -224,6 +234,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD3595D4-98DB-4287-B599-19A95C005976}" name="Table1" displayName="Table1" ref="A1:D2" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{DD3595D4-98DB-4287-B599-19A95C005976}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{F496841C-EFF1-41FD-AA83-C6DEC73A3375}" name="id"/>
+    <tableColumn id="2" xr3:uid="{2144077A-6AD5-428E-B68E-1797FAFF2AE4}" name="name"/>
+    <tableColumn id="3" xr3:uid="{73219B67-BDFC-469F-969F-0A3C9B36A525}" name="filename"/>
+    <tableColumn id="4" xr3:uid="{70C3642C-AA66-4982-BF5E-9C998534D13D}" name="caption"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -491,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
@@ -499,10 +522,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34.140625" customWidth="1"/>
@@ -743,14 +766,14 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="64.140625" style="1" customWidth="1"/>
@@ -808,7 +831,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,6 +979,57 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F785DB8B-55D3-48F8-994B-1E1D4064B752}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>50120</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{85ca8af4-763a-45c2-80ae-a5ca1b80bddc}" enabled="1" method="Standard" siteId="{06cdaf09-14f0-4cd1-8ac0-7bfed707a82c}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Updated embed generated with report selection feature
</commit_message>
<xml_diff>
--- a/samples/PowerBi/EmbedYourPBIApp/PBIPayloadGenerator/input.xlsx
+++ b/samples/PowerBi/EmbedYourPBIApp/PBIPayloadGenerator/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ys\Git\Other\BCTech\samples\PowerBi\EmbedYourPBIApp\PBIPayloadGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CFBE67E-C544-4C52-8342-5AD07D3D6ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6F98DD-AA7D-40A5-A5B6-BD06A8B77612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13650" yWindow="3240" windowWidth="23250" windowHeight="12450" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11796" yWindow="17172" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Namespace" sheetId="5" r:id="rId1"/>
@@ -59,18 +59,12 @@
     <t>Financial Overview</t>
   </si>
   <si>
-    <t>PBIReportId</t>
-  </si>
-  <si>
     <t>PBIReportName</t>
   </si>
   <si>
     <t>The financial overview page shows you all the possible ways you can analyze your sales, e.g. Sales summary, Sales pipeline, Sales leaderboard, Sales activity</t>
   </si>
   <si>
-    <t>061ce0f5-3918-44ee-b820-a8d0d384fb2e</t>
-  </si>
-  <si>
     <t>Financial overview</t>
   </si>
   <si>
@@ -158,13 +152,19 @@
     <t>Namespace</t>
   </si>
   <si>
-    <t>Microsoft.PowerBIApps</t>
-  </si>
-  <si>
     <t>Power BI Finance App - Objects</t>
   </si>
   <si>
     <t>PowerBIFinanceObjects.PermissionSet</t>
+  </si>
+  <si>
+    <t>PBIReportIdFieldName</t>
+  </si>
+  <si>
+    <t>Finance Report Id</t>
+  </si>
+  <si>
+    <t>Microsoft.Finance.PowerBIReports</t>
   </si>
 </sst>
 </file>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3EBBDE8-F668-4FEF-BBF8-181EE1A44204}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,12 +563,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -583,14 +583,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A2"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
@@ -612,22 +612,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>11</v>
-      </c>
       <c r="G1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -650,16 +650,16 @@
         <v>About Financial Overview</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -675,23 +675,23 @@
         <v>PBIIncomeStatementbyMonth.Page</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" ref="E3:E7" si="2">_xlfn.CONCAT("About ",D3)</f>
         <v>About Income Statement by Month</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -707,23 +707,23 @@
         <v>PBIBalanceSheetbyMonth.Page</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" si="2"/>
         <v>About Balance Sheet by Month</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -739,23 +739,23 @@
         <v>PBIBudgetComparison.Page</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" si="2"/>
         <v>About Budget Comparison</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="I5" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -771,23 +771,23 @@
         <v>PBILiquidityKPIs.Page</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" si="2"/>
         <v>About Liquidity KPIs</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -803,23 +803,23 @@
         <v>PBIProfitability.Page</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="2"/>
         <v>About Profitability</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -859,13 +859,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -873,19 +873,19 @@
         <v>50140</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -913,24 +913,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="str">
         <f t="shared" ref="B2:B7" si="0">_xlfn.CONCAT("PBI",SUBSTITUTE(C2," ",""))</f>
@@ -944,102 +944,102 @@
         <v>PBIFinancialOverview</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="str">
         <f t="shared" si="0"/>
         <v>PBIIncomeStatementbyMonth</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D7" si="1">B3</f>
         <v>PBIIncomeStatementbyMonth</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>PBIBalanceSheetbyMonth</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="1"/>
         <v>PBIBalanceSheetbyMonth</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>PBIBudgetComparison</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="1"/>
         <v>PBIBudgetComparison</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>PBILiquidityKPIs</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="1"/>
         <v>PBILiquidityKPIs</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>PBIProfitability</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="1"/>
         <v>PBIProfitability</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1052,7 +1052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F785DB8B-55D3-48F8-994B-1E1D4064B752}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
@@ -1078,10 +1078,10 @@
         <v>50120</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated report id and page code
</commit_message>
<xml_diff>
--- a/samples/PowerBi/EmbedYourPBIApp/PBIPayloadGenerator/input.xlsx
+++ b/samples/PowerBi/EmbedYourPBIApp/PBIPayloadGenerator/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ys\Git\Other\BCTech\samples\PowerBi\EmbedYourPBIApp\PBIPayloadGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAC32AC-D123-4647-8DAB-940E22674F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32EEC67-AA66-4FC0-B4BD-F2819360A599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10905" yWindow="3270" windowWidth="23250" windowHeight="12450" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3015" yWindow="7980" windowWidth="23250" windowHeight="12450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Namespace" sheetId="5" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -65,9 +65,6 @@
     <t>The financial overview page shows you all the possible ways you can analyze your sales, e.g. Sales summary, Sales pipeline, Sales leaderboard, Sales activity</t>
   </si>
   <si>
-    <t>Financial overview</t>
-  </si>
-  <si>
     <t>caption</t>
   </si>
   <si>
@@ -128,21 +125,6 @@
     <t>PBIReportPage</t>
   </si>
   <si>
-    <t>ReportSectionf72eb4d7e5e35db3b283</t>
-  </si>
-  <si>
-    <t>ReportSection6a30609896651f006f0f</t>
-  </si>
-  <si>
-    <t>ReportSection64d670dfa9da1a5b7033</t>
-  </si>
-  <si>
-    <t>ReportSection6838cf9cda361d088e0a</t>
-  </si>
-  <si>
-    <t>ReportSectionbb4917d9edb6d427282c</t>
-  </si>
-  <si>
     <t>Namespace</t>
   </si>
   <si>
@@ -170,7 +152,7 @@
     <t>Microsoft.Finance.RoleCenters</t>
   </si>
   <si>
-    <t>04fa320747962435bf38</t>
+    <t>Finance App</t>
   </si>
 </sst>
 </file>
@@ -569,12 +551,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -589,9 +571,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,22 +600,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>9</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -659,13 +641,13 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I2" s="2" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -681,7 +663,7 @@
         <v>IncomeStatementbyMonth.Page</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" ref="E3:E7" si="2">_xlfn.CONCAT("About ",D3)</f>
@@ -691,13 +673,13 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I3" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -713,7 +695,7 @@
         <v>BalanceSheetbyMonth.Page</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" si="2"/>
@@ -723,13 +705,13 @@
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -745,7 +727,7 @@
         <v>BudgetComparison.Page</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" si="2"/>
@@ -755,13 +737,13 @@
         <v>5</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I5" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -777,7 +759,7 @@
         <v>LiquidityKPIs.Page</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" si="2"/>
@@ -787,13 +769,13 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -809,7 +791,7 @@
         <v>Profitability.Page</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="2"/>
@@ -819,13 +801,13 @@
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="I7" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -866,16 +848,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -883,22 +865,22 @@
         <v>50140</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -912,7 +894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279D5BCD-102B-4F28-B1A5-95C97D1C61B4}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2:D7"/>
     </sheetView>
@@ -928,24 +910,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>20</v>
-      </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>C2</f>
@@ -959,102 +941,102 @@
         <v>Financial Overview</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="str">
         <f t="shared" ref="B3:B7" si="0">C3</f>
         <v>Income Statement by Month</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D7" si="1">B3</f>
         <v>Income Statement by Month</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Balance Sheet by Month</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="1"/>
         <v>Balance Sheet by Month</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Budget Comparison</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="1"/>
         <v>Budget Comparison</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Liquidity KPIs</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="1"/>
         <v>Liquidity KPIs</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Profitability</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="1"/>
         <v>Profitability</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1093,10 +1075,10 @@
         <v>50120</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Updated report id and page code"
This reverts commit 7132a7995cbbb758094b37b7773e0810940343bb.
</commit_message>
<xml_diff>
--- a/samples/PowerBi/EmbedYourPBIApp/PBIPayloadGenerator/input.xlsx
+++ b/samples/PowerBi/EmbedYourPBIApp/PBIPayloadGenerator/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ys\Git\Other\BCTech\samples\PowerBi\EmbedYourPBIApp\PBIPayloadGenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32EEC67-AA66-4FC0-B4BD-F2819360A599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAC32AC-D123-4647-8DAB-940E22674F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3015" yWindow="7980" windowWidth="23250" windowHeight="12450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10905" yWindow="3270" windowWidth="23250" windowHeight="12450" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Namespace" sheetId="5" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
@@ -65,6 +65,9 @@
     <t>The financial overview page shows you all the possible ways you can analyze your sales, e.g. Sales summary, Sales pipeline, Sales leaderboard, Sales activity</t>
   </si>
   <si>
+    <t>Financial overview</t>
+  </si>
+  <si>
     <t>caption</t>
   </si>
   <si>
@@ -125,6 +128,21 @@
     <t>PBIReportPage</t>
   </si>
   <si>
+    <t>ReportSectionf72eb4d7e5e35db3b283</t>
+  </si>
+  <si>
+    <t>ReportSection6a30609896651f006f0f</t>
+  </si>
+  <si>
+    <t>ReportSection64d670dfa9da1a5b7033</t>
+  </si>
+  <si>
+    <t>ReportSection6838cf9cda361d088e0a</t>
+  </si>
+  <si>
+    <t>ReportSectionbb4917d9edb6d427282c</t>
+  </si>
+  <si>
     <t>Namespace</t>
   </si>
   <si>
@@ -152,7 +170,7 @@
     <t>Microsoft.Finance.RoleCenters</t>
   </si>
   <si>
-    <t>Finance App</t>
+    <t>04fa320747962435bf38</t>
   </si>
 </sst>
 </file>
@@ -551,12 +569,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -571,9 +589,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,22 +618,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -641,13 +659,13 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -663,7 +681,7 @@
         <v>IncomeStatementbyMonth.Page</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" ref="E3:E7" si="2">_xlfn.CONCAT("About ",D3)</f>
@@ -673,13 +691,13 @@
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -695,7 +713,7 @@
         <v>BalanceSheetbyMonth.Page</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" si="2"/>
@@ -705,13 +723,13 @@
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -727,7 +745,7 @@
         <v>BudgetComparison.Page</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" si="2"/>
@@ -737,13 +755,13 @@
         <v>5</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -759,7 +777,7 @@
         <v>LiquidityKPIs.Page</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" si="2"/>
@@ -769,13 +787,13 @@
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -791,7 +809,7 @@
         <v>Profitability.Page</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" si="2"/>
@@ -801,13 +819,13 @@
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -848,16 +866,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -865,22 +883,22 @@
         <v>50140</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -894,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{279D5BCD-102B-4F28-B1A5-95C97D1C61B4}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D2" sqref="D2:D7"/>
     </sheetView>
@@ -910,24 +928,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>C2</f>
@@ -941,102 +959,102 @@
         <v>Financial Overview</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="str">
         <f t="shared" ref="B3:B7" si="0">C3</f>
         <v>Income Statement by Month</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D7" si="1">B3</f>
         <v>Income Statement by Month</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Balance Sheet by Month</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="1"/>
         <v>Balance Sheet by Month</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Budget Comparison</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="1"/>
         <v>Budget Comparison</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Liquidity KPIs</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="1"/>
         <v>Liquidity KPIs</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>Profitability</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="1"/>
         <v>Profitability</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1075,10 +1093,10 @@
         <v>50120</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>